<commit_message>
Alteração: leitura da planilha via link OneDrive
</commit_message>
<xml_diff>
--- a/BASE PARA DASH TESTE.xlsx
+++ b/BASE PARA DASH TESTE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mtechdisplays-my.sharepoint.com/personal/pcp_mtechdisplays_com_br/Documents/DASH_MTECH/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="8_{CF940A7D-B2C1-4B5C-85B5-37B847805C75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E9B1FC7-4744-4743-AB35-50D5D883BF88}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="8_{CF940A7D-B2C1-4B5C-85B5-37B847805C75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DB2CC1D-BBB5-4042-8817-F09D6597AF5B}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1F4BD7C2-DFC7-41C6-8F07-66FC27B5E6F6}"/>
   </bookViews>
@@ -1852,8 +1852,8 @@
   </sheetPr>
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2132,7 +2132,7 @@
         <f>G2</f>
         <v>Canaleta J Base/testeira</v>
       </c>
-      <c r="B10" s="30">
+      <c r="B10" s="32">
         <f>ROUNDDOWN(($H$5-$H$6)/$H$4,0)</f>
         <v>815</v>
       </c>

</xml_diff>